<commit_message>
-SAdding and Making 2nd Examination Timetable
</commit_message>
<xml_diff>
--- a/timeTableManagement.xlsx
+++ b/timeTableManagement.xlsx
@@ -721,7 +721,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="5">
-        <v>44989</v>
+        <v>45019</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
@@ -738,7 +738,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="5">
-        <v>44990</v>
+        <v>45020</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
@@ -755,7 +755,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="5">
-        <v>44991</v>
+        <v>45021</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
@@ -773,7 +773,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="5">
-        <v>44992</v>
+        <v>45022</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>15</v>
@@ -791,7 +791,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="5">
-        <v>44993</v>
+        <v>45023</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>16</v>
@@ -809,7 +809,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="5">
-        <v>44994</v>
+        <v>45024</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>17</v>
@@ -826,7 +826,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="1.2913385826771653" right="0.81889763779527569" top="1.1850393700787398" bottom="0.75196850393700776" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>